<commit_message>
feat(xlspython): modify all sheets methods so that it is now possible to apply a sheet method on multiple sheets. Add also an indicator of percentage of completion for all methods which acts on multiple tabs or files.
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_cmd_column_set_answer.xlsx
+++ b/fichiers_xls/test_cmd_column_set_answer.xlsx
@@ -462,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -497,21 +497,26 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
           <t>hen</t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr"/>
-      <c r="E2" s="3" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr"/>
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>henri</t>
         </is>
       </c>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>les boulets</t>
         </is>
       </c>
-      <c r="G2" s="3" t="inlineStr">
+      <c r="H2" s="3" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -528,25 +533,30 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
           <t>hen</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="E3" s="3" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>henri</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="G3" s="3" t="inlineStr">
         <is>
           <t>les boulets</t>
         </is>
       </c>
-      <c r="G3" s="3" t="inlineStr">
+      <c r="H3" s="3" t="inlineStr">
         <is>
           <t>9</t>
         </is>
@@ -563,25 +573,30 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
           <t>je</t>
         </is>
       </c>
-      <c r="D4" s="3" t="inlineStr">
+      <c r="E4" s="3" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E4" s="3" t="inlineStr">
+      <c r="F4" s="3" t="inlineStr">
         <is>
           <t>le smaaaaaaaaaaaaaaaaaaaaaaall</t>
         </is>
       </c>
-      <c r="F4" s="3" t="inlineStr">
+      <c r="G4" s="3" t="inlineStr">
         <is>
           <t>les boulets</t>
         </is>
       </c>
-      <c r="G4" s="3" t="inlineStr">
+      <c r="H4" s="3" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -598,21 +613,26 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>group1</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
           <t>je</t>
         </is>
       </c>
-      <c r="D5" s="3" t="inlineStr"/>
-      <c r="E5" s="3" t="inlineStr">
+      <c r="E5" s="3" t="inlineStr"/>
+      <c r="F5" s="3" t="inlineStr">
         <is>
           <t>le smaaaaaaaaaaaaaaaaaaaaaaall</t>
         </is>
       </c>
-      <c r="F5" s="3" t="inlineStr">
+      <c r="G5" s="3" t="inlineStr">
         <is>
           <t>les boulets</t>
         </is>
       </c>
-      <c r="G5" s="3" t="inlineStr">
+      <c r="H5" s="3" t="inlineStr">
         <is>
           <t>10</t>
         </is>
@@ -627,19 +647,24 @@
       <c r="B6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
       <c r="D6" s="3" t="inlineStr"/>
-      <c r="E6" s="3" t="inlineStr">
+      <c r="E6" s="3" t="inlineStr"/>
+      <c r="F6" s="3" t="inlineStr">
         <is>
           <t>henri</t>
         </is>
       </c>
-      <c r="F6" s="3" t="inlineStr">
+      <c r="G6" s="3" t="inlineStr">
         <is>
           <t>les pelicans</t>
         </is>
       </c>
-      <c r="G6" s="3" t="n"/>
+      <c r="H6" s="3" t="n"/>
     </row>
     <row r="7" ht="16.05" customHeight="1" s="4">
       <c r="A7" s="3" t="inlineStr">
@@ -650,19 +675,24 @@
       <c r="B7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
       <c r="D7" s="3" t="inlineStr"/>
-      <c r="E7" s="3" t="inlineStr">
+      <c r="E7" s="3" t="inlineStr"/>
+      <c r="F7" s="3" t="inlineStr">
         <is>
           <t>henri</t>
         </is>
       </c>
-      <c r="F7" s="3" t="inlineStr">
+      <c r="G7" s="3" t="inlineStr">
         <is>
           <t>les pelicans</t>
         </is>
       </c>
-      <c r="G7" s="3" t="n"/>
+      <c r="H7" s="3" t="n"/>
     </row>
     <row r="8" ht="16.05" customHeight="1" s="4">
       <c r="A8" s="3" t="inlineStr">
@@ -673,19 +703,24 @@
       <c r="B8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
       <c r="D8" s="3" t="inlineStr"/>
-      <c r="E8" s="3" t="inlineStr">
+      <c r="E8" s="3" t="inlineStr"/>
+      <c r="F8" s="3" t="inlineStr">
         <is>
           <t>le smaaaaaaaaaaaaaaaaaaaaaaall</t>
         </is>
       </c>
-      <c r="F8" s="3" t="inlineStr">
+      <c r="G8" s="3" t="inlineStr">
         <is>
           <t>les pelicans</t>
         </is>
       </c>
-      <c r="G8" s="3" t="n"/>
+      <c r="H8" s="3" t="n"/>
     </row>
     <row r="9" ht="16.05" customHeight="1" s="4">
       <c r="A9" s="3" t="inlineStr">
@@ -696,15 +731,20 @@
       <c r="B9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
       <c r="D9" s="3" t="inlineStr"/>
       <c r="E9" s="3" t="inlineStr"/>
-      <c r="F9" s="3" t="inlineStr">
+      <c r="F9" s="3" t="inlineStr"/>
+      <c r="G9" s="3" t="inlineStr">
         <is>
           <t>les pelicans</t>
         </is>
       </c>
-      <c r="G9" s="3" t="n"/>
+      <c r="H9" s="3" t="n"/>
     </row>
     <row r="10" ht="16.05" customHeight="1" s="4">
       <c r="A10" s="3" t="inlineStr">
@@ -717,7 +757,8 @@
       <c r="D10" s="3" t="inlineStr"/>
       <c r="E10" s="3" t="inlineStr"/>
       <c r="F10" s="3" t="inlineStr"/>
-      <c r="G10" s="3" t="n"/>
+      <c r="G10" s="3" t="inlineStr"/>
+      <c r="H10" s="3" t="n"/>
     </row>
     <row r="11" ht="16.05" customHeight="1" s="4">
       <c r="A11" s="3" t="inlineStr">
@@ -728,15 +769,20 @@
       <c r="B11" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
       <c r="D11" s="3" t="inlineStr"/>
       <c r="E11" s="3" t="inlineStr"/>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr"/>
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>les pelicans</t>
         </is>
       </c>
-      <c r="G11" s="3" t="n"/>
+      <c r="H11" s="3" t="n"/>
     </row>
     <row r="12" ht="16.05" customHeight="1" s="4">
       <c r="A12" s="3" t="inlineStr">
@@ -747,15 +793,20 @@
       <c r="B12" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
       <c r="D12" s="3" t="inlineStr"/>
       <c r="E12" s="3" t="inlineStr"/>
-      <c r="F12" s="3" t="inlineStr">
+      <c r="F12" s="3" t="inlineStr"/>
+      <c r="G12" s="3" t="inlineStr">
         <is>
           <t>les pelicans</t>
         </is>
       </c>
-      <c r="G12" s="3" t="n"/>
+      <c r="H12" s="3" t="n"/>
     </row>
     <row r="13" ht="16.05" customHeight="1" s="4">
       <c r="A13" s="3" t="inlineStr">
@@ -766,15 +817,20 @@
       <c r="B13" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
       <c r="D13" s="3" t="inlineStr"/>
       <c r="E13" s="3" t="inlineStr"/>
-      <c r="F13" s="3" t="inlineStr">
+      <c r="F13" s="3" t="inlineStr"/>
+      <c r="G13" s="3" t="inlineStr">
         <is>
           <t>les pelicans</t>
         </is>
       </c>
-      <c r="G13" s="3" t="n"/>
+      <c r="H13" s="3" t="n"/>
     </row>
     <row r="14" ht="16.05" customHeight="1" s="4">
       <c r="A14" s="5" t="inlineStr">
@@ -785,19 +841,24 @@
       <c r="B14" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
       <c r="D14" s="3" t="inlineStr"/>
-      <c r="E14" s="3" t="inlineStr">
+      <c r="E14" s="3" t="inlineStr"/>
+      <c r="F14" s="3" t="inlineStr">
         <is>
           <t>le smaaaaaaaaaaaaaaaaaaaaaaall</t>
         </is>
       </c>
-      <c r="F14" s="3" t="inlineStr">
+      <c r="G14" s="3" t="inlineStr">
         <is>
           <t>les pelicans</t>
         </is>
       </c>
-      <c r="G14" s="3" t="n"/>
+      <c r="H14" s="3" t="n"/>
     </row>
     <row r="15" ht="16.05" customHeight="1" s="4">
       <c r="A15" s="5" t="inlineStr">
@@ -808,19 +869,24 @@
       <c r="B15" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>group2</t>
+        </is>
+      </c>
       <c r="D15" s="3" t="inlineStr"/>
-      <c r="E15" s="3" t="inlineStr">
+      <c r="E15" s="3" t="inlineStr"/>
+      <c r="F15" s="3" t="inlineStr">
         <is>
           <t>henri</t>
         </is>
       </c>
-      <c r="F15" s="3" t="inlineStr">
+      <c r="G15" s="3" t="inlineStr">
         <is>
           <t>les pelicans</t>
         </is>
       </c>
-      <c r="G15" s="3" t="n"/>
+      <c r="H15" s="3" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>